<commit_message>
Added Testpiece in STLs
</commit_message>
<xml_diff>
--- a/0_General Data/Manuals/Sources/Print Settings.xlsx
+++ b/0_General Data/Manuals/Sources/Print Settings.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LC\Documents\Git\Open-Wing\0_General Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LC\Documents\Git\Open-Wing\0_General Data\Manuals\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838268CA-25B2-435E-A688-5033C2B2CA06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0353A6-1301-41E1-ACA0-D2A71846EA29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19176" windowHeight="7980" xr2:uid="{F8FDE17F-D961-4D39-891A-0CD456EB19CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Printsettings_General" sheetId="4" r:id="rId1"/>
     <sheet name="Printsettings_V3_Slope" sheetId="2" r:id="rId2"/>
+    <sheet name="Printsettings_V5_Community" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="84">
   <si>
     <t>Width</t>
   </si>
@@ -245,6 +246,39 @@
   </si>
   <si>
     <t>37g</t>
+  </si>
+  <si>
+    <t>34g</t>
+  </si>
+  <si>
+    <t>0.35mm</t>
+  </si>
+  <si>
+    <t>20g</t>
+  </si>
+  <si>
+    <t>203g</t>
+  </si>
+  <si>
+    <t>139g</t>
+  </si>
+  <si>
+    <t>191g</t>
+  </si>
+  <si>
+    <t>164g</t>
+  </si>
+  <si>
+    <t>Infill before walls</t>
+  </si>
+  <si>
+    <t>OFF!</t>
+  </si>
+  <si>
+    <t>75g</t>
+  </si>
+  <si>
+    <t>Complete 24g</t>
   </si>
 </sst>
 </file>
@@ -636,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F06A536-0F68-4E3F-915E-6B8B0E70DAA9}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B19"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -733,57 +767,65 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B13" s="6">
         <v>-0.35</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-    </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>36</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B16" s="3">
         <v>0.4</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-    </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>36</v>
-      </c>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B20" s="3">
         <v>4</v>
       </c>
     </row>
@@ -1655,4 +1697,865 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE77A36C-5D50-4E6F-96A7-6DC7B25B3D0B}">
+  <dimension ref="A1:I45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="4.77734375" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" customWidth="1"/>
+    <col min="7" max="7" width="5.77734375" customWidth="1"/>
+    <col min="8" max="8" width="7.77734375" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2</v>
+      </c>
+      <c r="H2" s="3">
+        <v>2</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3">
+        <v>2</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="G11" s="3">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3">
+        <v>2</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3">
+        <v>2</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0.24</v>
+      </c>
+      <c r="G14" s="3">
+        <v>2</v>
+      </c>
+      <c r="H14" s="3">
+        <v>2</v>
+      </c>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3">
+        <v>2</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="G20" s="3">
+        <v>2</v>
+      </c>
+      <c r="H20" s="3">
+        <v>2</v>
+      </c>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3">
+        <v>3</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0.36</v>
+      </c>
+      <c r="G21" s="3">
+        <v>2</v>
+      </c>
+      <c r="H21" s="3">
+        <v>2</v>
+      </c>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="3">
+        <v>1</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="G24" s="3">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3">
+        <v>2</v>
+      </c>
+      <c r="F26" s="6">
+        <v>0.24</v>
+      </c>
+      <c r="G26" s="3">
+        <v>2</v>
+      </c>
+      <c r="H26" s="3">
+        <v>2</v>
+      </c>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3">
+        <v>3</v>
+      </c>
+      <c r="F27" s="6">
+        <v>0.36</v>
+      </c>
+      <c r="G27" s="3">
+        <v>2</v>
+      </c>
+      <c r="H27" s="3">
+        <v>2</v>
+      </c>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="4"/>
+      <c r="D30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="3">
+        <v>1</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0.03</v>
+      </c>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="6">
+        <v>0.12</v>
+      </c>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3">
+        <v>2</v>
+      </c>
+      <c r="F33" s="6">
+        <v>0.24</v>
+      </c>
+      <c r="G33" s="3">
+        <v>2</v>
+      </c>
+      <c r="H33" s="3">
+        <v>2</v>
+      </c>
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3">
+        <v>100</v>
+      </c>
+      <c r="F34" s="6"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1</v>
+      </c>
+      <c r="F36" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="3"/>
+      <c r="C37" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E39" s="3">
+        <v>1</v>
+      </c>
+      <c r="F39" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="3">
+        <v>1</v>
+      </c>
+      <c r="F42" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="G42" s="3">
+        <v>2</v>
+      </c>
+      <c r="H42" s="3">
+        <v>2</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E43" s="3">
+        <v>50</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E45" s="3">
+        <v>2</v>
+      </c>
+      <c r="F45" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="G45" s="3">
+        <v>4</v>
+      </c>
+      <c r="H45" s="3">
+        <v>4</v>
+      </c>
+      <c r="I45" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>